<commit_message>
first version of localcorrmodel
</commit_message>
<xml_diff>
--- a/QuantLibXL/StandaloneExamples/Analytics/YieldTermStructures.xlsx
+++ b/QuantLibXL/StandaloneExamples/Analytics/YieldTermStructures.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="14220" windowHeight="8835"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="14220" windowHeight="8832"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -169,10 +169,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
-    <numFmt numFmtId="172" formatCode="ddd\,\ d\-mmm\-yyyy"/>
-    <numFmt numFmtId="173" formatCode="0.0000"/>
-    <numFmt numFmtId="174" formatCode="0.000000000"/>
-    <numFmt numFmtId="175" formatCode="0.0000%"/>
+    <numFmt numFmtId="164" formatCode="ddd\,\ d\-mmm\-yyyy"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.000000000"/>
+    <numFmt numFmtId="167" formatCode="0.0000%"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -182,10 +182,12 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -334,11 +336,11 @@
   <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="172" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="173" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="174" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="175" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="175" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -352,24 +354,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="173" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="174" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="174" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="174" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -379,10 +381,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="3" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -701,35 +703,35 @@
   <dimension ref="A1:U37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" style="1" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="7" style="1" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="4.33203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="2.85546875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="2.88671875" style="1" customWidth="1"/>
     <col min="16" max="16" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="2" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="20" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="1"/>
+    <col min="22" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D1" s="30" t="s">
         <v>0</v>
       </c>
@@ -744,7 +746,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D2" s="33" t="s">
         <v>2</v>
       </c>
@@ -759,7 +761,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D3" s="33" t="s">
         <v>5</v>
       </c>
@@ -768,13 +770,13 @@
       </c>
       <c r="K3" s="42">
         <f ca="1">_xll.qlTermStructureReferenceDate($D$5)</f>
-        <v>41772</v>
+        <v>43073</v>
       </c>
       <c r="L3" s="35" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D4" s="36" t="s">
         <v>3</v>
       </c>
@@ -783,16 +785,16 @@
       </c>
       <c r="K4" s="42">
         <f ca="1">_xll.qlTermStructureMaxDate($D$5)</f>
-        <v>52730</v>
+        <v>54030</v>
       </c>
       <c r="L4" s="35" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D5" s="1" t="str">
         <f ca="1">_xll.qlInterpolatedYieldCurve(,$D$8:$D$28,IF($D$3=$E$7,E8:E28,IF($D$3=$F$7,F8:F28,G8:G28)),$D$2,$D$1,,,D3,D4)</f>
-        <v>obj_000dd#0002</v>
+        <v>obj_00081#0023</v>
       </c>
       <c r="K5" s="36" t="e">
         <f ca="1">_xll.qlTermStructureSettlementDays($D$5)</f>
@@ -802,7 +804,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>12</v>
       </c>
@@ -845,7 +847,7 @@
       <c r="T7" s="7"/>
       <c r="U7" s="7"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <f ca="1">_xll.qlDayCounterYearFraction($D$1,$D$8,D8)</f>
         <v>0</v>
@@ -856,7 +858,7 @@
       </c>
       <c r="D8" s="14">
         <f ca="1">_xll.qlCalendarAdvance($D$2,TODAY(),"2D")</f>
-        <v>41772</v>
+        <v>43073</v>
       </c>
       <c r="E8" s="15">
         <f ca="1">EXP(-F8*A8)</f>
@@ -880,7 +882,7 @@
       </c>
       <c r="K8" s="14">
         <f t="array" aca="1" ref="K8:K28" ca="1">_xll.qlInterpolatedYieldCurveDates($D$5)</f>
-        <v>41772</v>
+        <v>43073</v>
       </c>
       <c r="L8" s="15">
         <f t="array" aca="1" ref="L8:L28" ca="1">_xll.qlYieldTSDiscount(D$5,$D$8:$D$28)</f>
@@ -916,25 +918,25 @@
       </c>
       <c r="U8" s="5"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="18">
         <f ca="1">_xll.qlDayCounterYearFraction($D$1,$D$8,D9)</f>
-        <v>0.25205479452054796</v>
+        <v>0.24931506849315069</v>
       </c>
       <c r="B9" s="19">
         <f ca="1">A9-A8</f>
-        <v>0.25205479452054796</v>
+        <v>0.24931506849315069</v>
       </c>
       <c r="C9" s="43" t="s">
         <v>18</v>
       </c>
       <c r="D9" s="20">
         <f ca="1">_xll.qlCalendarAdvance($D$2,$D$8,C9)</f>
-        <v>41864</v>
+        <v>43164</v>
       </c>
       <c r="E9" s="21">
         <f t="shared" ref="E9:E28" ca="1" si="5">EXP(-F9*A9)</f>
-        <v>0.98996846313427345</v>
+        <v>0.99007695877372148</v>
       </c>
       <c r="F9" s="22">
         <f ca="1">SUMPRODUCT($B$9:B9,$G$9:G9)/A9</f>
@@ -949,19 +951,19 @@
       </c>
       <c r="J9" s="19">
         <f ca="1"/>
-        <v>0.25205479452054796</v>
+        <v>0.24931506849315069</v>
       </c>
       <c r="K9" s="20">
         <f ca="1"/>
-        <v>41864</v>
+        <v>43164</v>
       </c>
       <c r="L9" s="21">
         <f ca="1"/>
-        <v>0.98996846313427345</v>
+        <v>0.99007695877372148</v>
       </c>
       <c r="M9" s="40">
         <f ca="1"/>
-        <v>4.0000000000000112E-2</v>
+        <v>3.9999999999999834E-2</v>
       </c>
       <c r="N9" s="23">
         <f ca="1">_xll.qlYieldTSForwardRate(D$5,$D9,$D9,$D$1,"continuous","annual")</f>
@@ -981,7 +983,7 @@
       </c>
       <c r="S9" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>1.1102230246251565E-16</v>
+        <v>-1.6653345369377348E-16</v>
       </c>
       <c r="T9" s="5">
         <f t="shared" ca="1" si="4"/>
@@ -989,29 +991,29 @@
       </c>
       <c r="U9" s="5"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="18">
         <f ca="1">_xll.qlDayCounterYearFraction($D$1,$D$8,D10)</f>
-        <v>0.50410958904109593</v>
+        <v>0.49863013698630138</v>
       </c>
       <c r="B10" s="19">
         <f t="shared" ref="B10:B28" ca="1" si="6">A10-A9</f>
-        <v>0.25205479452054796</v>
+        <v>0.24931506849315069</v>
       </c>
       <c r="C10" s="43" t="s">
         <v>19</v>
       </c>
       <c r="D10" s="20">
         <f ca="1">_xll.qlCalendarAdvance($D$2,$D$8,C10)</f>
-        <v>41956</v>
+        <v>43255</v>
       </c>
       <c r="E10" s="21">
         <f t="shared" ca="1" si="5"/>
-        <v>0.98251090543941544</v>
+        <v>0.98269935025787736</v>
       </c>
       <c r="F10" s="22">
         <f ca="1">SUMPRODUCT($B$9:B10,$G$9:G10)/A10</f>
-        <v>3.4999999999999996E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="G10" s="23">
         <v>0.03</v>
@@ -1022,23 +1024,23 @@
       </c>
       <c r="J10" s="19">
         <f ca="1"/>
-        <v>0.50410958904109593</v>
+        <v>0.49863013698630138</v>
       </c>
       <c r="K10" s="20">
         <f ca="1"/>
-        <v>41956</v>
+        <v>43255</v>
       </c>
       <c r="L10" s="21">
         <f ca="1"/>
-        <v>0.98003755800043535</v>
+        <v>0.98025238429462136</v>
       </c>
       <c r="M10" s="40">
         <f ca="1"/>
-        <v>4.0000000000000042E-2</v>
+        <v>3.9999999999999786E-2</v>
       </c>
       <c r="N10" s="23">
         <f ca="1">_xll.qlYieldTSForwardRate(D$5,$D10,$D10,$D$1,"continuous","annual")</f>
-        <v>3.5000000001384139E-2</v>
+        <v>3.49999999991637E-2</v>
       </c>
       <c r="P10" s="3">
         <f t="shared" ca="1" si="0"/>
@@ -1050,37 +1052,37 @@
       </c>
       <c r="R10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>-2.4733474389800891E-3</v>
+        <v>-2.4469659632559981E-3</v>
       </c>
       <c r="S10" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>5.0000000000000461E-3</v>
+        <v>4.9999999999997824E-3</v>
       </c>
       <c r="T10" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>5.0000000013841403E-3</v>
+        <v>4.9999999991637012E-3</v>
       </c>
       <c r="U10" s="5"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="18">
         <f ca="1">_xll.qlDayCounterYearFraction($D$1,$D$8,D11)</f>
-        <v>0.75616438356164384</v>
+        <v>0.75068493150684934</v>
       </c>
       <c r="B11" s="19">
         <f t="shared" ca="1" si="6"/>
-        <v>0.25205479452054791</v>
+        <v>0.25205479452054796</v>
       </c>
       <c r="C11" s="43" t="s">
         <v>20</v>
       </c>
       <c r="D11" s="20">
         <f ca="1">_xll.qlCalendarAdvance($D$2,$D$8,C11)</f>
-        <v>42048</v>
+        <v>43347</v>
       </c>
       <c r="E11" s="21">
         <f t="shared" ca="1" si="5"/>
-        <v>0.973881395367025</v>
+        <v>0.97406818505224613</v>
       </c>
       <c r="F11" s="22">
         <f ca="1">SUMPRODUCT($B$9:B11,$G$9:G11)/A11</f>
@@ -1095,23 +1097,23 @@
       </c>
       <c r="J11" s="19">
         <f ca="1"/>
-        <v>0.75616438356164384</v>
+        <v>0.75068493150684934</v>
       </c>
       <c r="K11" s="20">
         <f ca="1"/>
-        <v>42048</v>
+        <v>43347</v>
       </c>
       <c r="L11" s="21">
         <f ca="1"/>
-        <v>0.97265481107052165</v>
+        <v>0.97286801905105125</v>
       </c>
       <c r="M11" s="40">
         <f ca="1"/>
-        <v>3.6666666666666577E-2</v>
+        <v>3.6642335766423256E-2</v>
       </c>
       <c r="N11" s="23">
         <f ca="1">_xll.qlYieldTSForwardRate(D$5,$D11,$D11,$D$1,"continuous","annual")</f>
-        <v>3.2500000000853957E-2</v>
+        <v>3.2499999998633518E-2</v>
       </c>
       <c r="P11" s="3">
         <f t="shared" ca="1" si="0"/>
@@ -1123,41 +1125,41 @@
       </c>
       <c r="R11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>-1.2265842965033524E-3</v>
+        <v>-1.20016600119488E-3</v>
       </c>
       <c r="S11" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>1.6666666666665803E-3</v>
+        <v>1.6423357664232599E-3</v>
       </c>
       <c r="T11" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>-2.4999999991460464E-3</v>
+        <v>-2.5000000013664855E-3</v>
       </c>
       <c r="U11" s="5"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="18">
         <f ca="1">_xll.qlDayCounterYearFraction($D$1,$D$8,D12)</f>
         <v>1</v>
       </c>
       <c r="B12" s="19">
         <f t="shared" ca="1" si="6"/>
-        <v>0.24383561643835616</v>
+        <v>0.24931506849315066</v>
       </c>
       <c r="C12" s="43" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="20">
         <f ca="1">_xll.qlCalendarAdvance($D$2,$D$8,C12)</f>
-        <v>42137</v>
+        <v>43438</v>
       </c>
       <c r="E12" s="21">
         <f t="shared" ca="1" si="5"/>
-        <v>0.9648993275676806</v>
+        <v>0.96488346633923783</v>
       </c>
       <c r="F12" s="22">
         <f ca="1">SUMPRODUCT($B$9:B12,$G$9:G12)/A12</f>
-        <v>3.5731506849315066E-2</v>
+        <v>3.5747945205479449E-2</v>
       </c>
       <c r="G12" s="23">
         <v>3.7999999999999999E-2</v>
@@ -1172,15 +1174,15 @@
       </c>
       <c r="K12" s="20">
         <f ca="1"/>
-        <v>42137</v>
+        <v>43438</v>
       </c>
       <c r="L12" s="21">
         <f ca="1"/>
-        <v>0.96438925539256326</v>
+        <v>0.96441567737794198</v>
       </c>
       <c r="M12" s="40">
         <f ca="1"/>
-        <v>3.6260273972602598E-2</v>
+        <v>3.6232876712328735E-2</v>
       </c>
       <c r="N12" s="23">
         <f ca="1">_xll.qlYieldTSForwardRate(D$5,$D12,$D12,$D$1,"continuous","annual")</f>
@@ -1196,11 +1198,11 @@
       </c>
       <c r="R12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>-5.100721751173376E-4</v>
+        <v>-4.6778896129584524E-4</v>
       </c>
       <c r="S12" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>5.2876712328753239E-4</v>
+        <v>4.8493150684928571E-4</v>
       </c>
       <c r="T12" s="5">
         <f t="shared" ca="1" si="4"/>
@@ -1208,29 +1210,29 @@
       </c>
       <c r="U12" s="5"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="18">
         <f ca="1">_xll.qlDayCounterYearFraction($D$1,$D$8,D13)</f>
-        <v>1.252054794520548</v>
+        <v>1.2465753424657535</v>
       </c>
       <c r="B13" s="19">
         <f t="shared" ca="1" si="6"/>
-        <v>0.25205479452054802</v>
+        <v>0.24657534246575352</v>
       </c>
       <c r="C13" s="43" t="s">
         <v>22</v>
       </c>
       <c r="D13" s="20">
         <f ca="1">_xll.qlCalendarAdvance($D$2,$D$8,C13)</f>
-        <v>42229</v>
+        <v>43528</v>
       </c>
       <c r="E13" s="21">
         <f t="shared" ca="1" si="5"/>
-        <v>0.95521990439147064</v>
+        <v>0.9554135850459009</v>
       </c>
       <c r="F13" s="22">
         <f ca="1">SUMPRODUCT($B$9:B13,$G$9:G13)/A13</f>
-        <v>3.6590809628008751E-2</v>
+        <v>3.6589010989010989E-2</v>
       </c>
       <c r="G13" s="23">
         <v>0.04</v>
@@ -1241,19 +1243,19 @@
       </c>
       <c r="J13" s="19">
         <f ca="1"/>
-        <v>1.252054794520548</v>
+        <v>1.2465753424657535</v>
       </c>
       <c r="K13" s="20">
         <f ca="1"/>
-        <v>42229</v>
+        <v>43528</v>
       </c>
       <c r="L13" s="21">
         <f ca="1"/>
-        <v>0.95519635131434666</v>
+        <v>0.95542143779257005</v>
       </c>
       <c r="M13" s="40">
         <f ca="1"/>
-        <v>3.6610503282275726E-2</v>
+        <v>3.6582417582417537E-2</v>
       </c>
       <c r="N13" s="23">
         <f ca="1">_xll.qlYieldTSForwardRate(D$5,$D13,$D13,$D$1,"continuous","annual")</f>
@@ -1269,11 +1271,11 @@
       </c>
       <c r="R13" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>-2.3553077123983357E-5</v>
+        <v>7.8527466691458159E-6</v>
       </c>
       <c r="S13" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>1.9693654266975114E-5</v>
+        <v>-6.5934065934525332E-6</v>
       </c>
       <c r="T13" s="5">
         <f t="shared" ca="1" si="4"/>
@@ -1281,10 +1283,10 @@
       </c>
       <c r="U13" s="5"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="18">
         <f ca="1">_xll.qlDayCounterYearFraction($D$1,$D$8,D14)</f>
-        <v>1.5041095890410958</v>
+        <v>1.4986301369863013</v>
       </c>
       <c r="B14" s="19">
         <f t="shared" ca="1" si="6"/>
@@ -1295,15 +1297,15 @@
       </c>
       <c r="D14" s="20">
         <f ca="1">_xll.qlCalendarAdvance($D$2,$D$8,C14)</f>
-        <v>42321</v>
+        <v>43620</v>
       </c>
       <c r="E14" s="21">
         <f t="shared" ca="1" si="5"/>
-        <v>0.9451609958690862</v>
+        <v>0.94535263697641692</v>
       </c>
       <c r="F14" s="22">
         <f ca="1">SUMPRODUCT($B$9:B14,$G$9:G14)/A14</f>
-        <v>3.7497267759562837E-2</v>
+        <v>3.7499085923217552E-2</v>
       </c>
       <c r="G14" s="23">
         <v>4.2000000000000003E-2</v>
@@ -1314,19 +1316,19 @@
       </c>
       <c r="J14" s="19">
         <f ca="1"/>
-        <v>1.5041095890410958</v>
+        <v>1.4986301369863013</v>
       </c>
       <c r="K14" s="20">
         <f ca="1"/>
-        <v>42321</v>
+        <v>43620</v>
       </c>
       <c r="L14" s="21">
         <f ca="1"/>
-        <v>0.94561426390212933</v>
+        <v>0.94583709241704839</v>
       </c>
       <c r="M14" s="40">
         <f ca="1"/>
-        <v>3.7178506375227689E-2</v>
+        <v>3.7157221206581409E-2</v>
       </c>
       <c r="N14" s="23">
         <f ca="1">_xll.qlYieldTSForwardRate(D$5,$D14,$D14,$D$1,"continuous","annual")</f>
@@ -1342,11 +1344,11 @@
       </c>
       <c r="R14" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>4.5326803304313046E-4</v>
+        <v>4.844554406314705E-4</v>
       </c>
       <c r="S14" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>-3.1876138433514778E-4</v>
+        <v>-3.4186471663614354E-4</v>
       </c>
       <c r="T14" s="5">
         <f t="shared" ca="1" si="4"/>
@@ -1354,29 +1356,29 @@
       </c>
       <c r="U14" s="5"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="18">
         <f ca="1">_xll.qlDayCounterYearFraction($D$1,$D$8,D15)</f>
-        <v>1.7616438356164383</v>
+        <v>1.7506849315068493</v>
       </c>
       <c r="B15" s="19">
         <f t="shared" ca="1" si="6"/>
-        <v>0.25753424657534252</v>
+        <v>0.25205479452054802</v>
       </c>
       <c r="C15" s="43" t="s">
         <v>24</v>
       </c>
       <c r="D15" s="20">
         <f ca="1">_xll.qlCalendarAdvance($D$2,$D$8,C15)</f>
-        <v>42415</v>
+        <v>43712</v>
       </c>
       <c r="E15" s="21">
         <f t="shared" ca="1" si="5"/>
-        <v>0.93451134979309036</v>
+        <v>0.93492621127243436</v>
       </c>
       <c r="F15" s="22">
         <f ca="1">SUMPRODUCT($B$9:B15,$G$9:G15)/A15</f>
-        <v>3.8447900466562983E-2</v>
+        <v>3.8435054773082941E-2</v>
       </c>
       <c r="G15" s="23">
         <v>4.3999999999999997E-2</v>
@@ -1387,23 +1389,23 @@
       </c>
       <c r="J15" s="19">
         <f ca="1"/>
-        <v>1.7616438356164383</v>
+        <v>1.7506849315068493</v>
       </c>
       <c r="K15" s="20">
         <f ca="1"/>
-        <v>42415</v>
+        <v>43712</v>
       </c>
       <c r="L15" s="21">
         <f ca="1"/>
-        <v>0.93544120283508514</v>
+        <v>0.93587698925550244</v>
       </c>
       <c r="M15" s="40">
         <f ca="1"/>
-        <v>3.7883359253499213E-2</v>
+        <v>3.7854460093896702E-2</v>
       </c>
       <c r="N15" s="23">
         <f ca="1">_xll.qlYieldTSForwardRate(D$5,$D15,$D15,$D$1,"continuous","annual")</f>
-        <v>4.2999999998820135E-2</v>
+        <v>4.3000000001040574E-2</v>
       </c>
       <c r="P15" s="3">
         <f t="shared" ca="1" si="0"/>
@@ -1415,41 +1417,41 @@
       </c>
       <c r="R15" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>9.2985304199477703E-4</v>
+        <v>9.5077798306808514E-4</v>
       </c>
       <c r="S15" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>-5.6454121306376975E-4</v>
+        <v>-5.8059467918623875E-4</v>
       </c>
       <c r="T15" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>-1.0000000011798627E-3</v>
+        <v>-9.9999999895942354E-4</v>
       </c>
       <c r="U15" s="5"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="18">
         <f ca="1">_xll.qlDayCounterYearFraction($D$1,$D$8,D16)</f>
-        <v>2.0027397260273974</v>
+        <v>2</v>
       </c>
       <c r="B16" s="19">
         <f t="shared" ca="1" si="6"/>
-        <v>0.24109589041095902</v>
+        <v>0.24931506849315066</v>
       </c>
       <c r="C16" s="43" t="s">
         <v>25</v>
       </c>
       <c r="D16" s="20">
         <f ca="1">_xll.qlCalendarAdvance($D$2,$D$8,C16)</f>
-        <v>42503</v>
+        <v>43803</v>
       </c>
       <c r="E16" s="21">
         <f t="shared" ca="1" si="5"/>
-        <v>0.9242044941531572</v>
+        <v>0.92426526576168044</v>
       </c>
       <c r="F16" s="22">
         <f ca="1">SUMPRODUCT($B$9:B16,$G$9:G16)/A16</f>
-        <v>3.9357045143638851E-2</v>
+        <v>3.9378082191780822E-2</v>
       </c>
       <c r="G16" s="23">
         <v>4.5999999999999999E-2</v>
@@ -1460,19 +1462,19 @@
       </c>
       <c r="J16" s="19">
         <f ca="1"/>
-        <v>2.0027397260273974</v>
+        <v>2</v>
       </c>
       <c r="K16" s="20">
         <f ca="1"/>
-        <v>42503</v>
+        <v>43803</v>
       </c>
       <c r="L16" s="21">
         <f ca="1"/>
-        <v>0.92557028651699003</v>
+        <v>0.92566665227536071</v>
       </c>
       <c r="M16" s="40">
         <f ca="1"/>
-        <v>3.8619699042407606E-2</v>
+        <v>3.8620547945205468E-2</v>
       </c>
       <c r="N16" s="23">
         <f ca="1">_xll.qlYieldTSForwardRate(D$5,$D16,$D16,$D$1,"continuous","annual")</f>
@@ -1488,11 +1490,11 @@
       </c>
       <c r="R16" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>1.3657923638328295E-3</v>
+        <v>1.4013865136802695E-3</v>
       </c>
       <c r="S16" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>-7.3734610123124544E-4</v>
+        <v>-7.5753424657535456E-4</v>
       </c>
       <c r="T16" s="5">
         <f t="shared" ca="1" si="4"/>
@@ -1500,29 +1502,29 @@
       </c>
       <c r="U16" s="5"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="18">
         <f ca="1">_xll.qlDayCounterYearFraction($D$1,$D$8,D17)</f>
-        <v>3.0082191780821916</v>
+        <v>3.0027397260273974</v>
       </c>
       <c r="B17" s="19">
         <f t="shared" ca="1" si="6"/>
-        <v>1.0054794520547943</v>
+        <v>1.0027397260273974</v>
       </c>
       <c r="C17" s="43" t="s">
         <v>26</v>
       </c>
       <c r="D17" s="20">
         <f ca="1">_xll.qlCalendarAdvance($D$2,$D$8,C17)</f>
-        <v>42870</v>
+        <v>44169</v>
       </c>
       <c r="E17" s="21">
         <f t="shared" ca="1" si="5"/>
-        <v>0.88065887373564533</v>
+        <v>0.88083260988141132</v>
       </c>
       <c r="F17" s="22">
         <f ca="1">SUMPRODUCT($B$9:B17,$G$9:G17)/A17</f>
-        <v>4.224590163934426E-2</v>
+        <v>4.2257299270072997E-2</v>
       </c>
       <c r="G17" s="23">
         <v>4.8000000000000001E-2</v>
@@ -1533,23 +1535,23 @@
       </c>
       <c r="J17" s="19">
         <f ca="1"/>
-        <v>3.0082191780821916</v>
+        <v>3.0027397260273974</v>
       </c>
       <c r="K17" s="20">
         <f ca="1"/>
-        <v>42870</v>
+        <v>44169</v>
       </c>
       <c r="L17" s="21">
         <f ca="1"/>
-        <v>0.8837356846892549</v>
+        <v>0.88393908836087254</v>
       </c>
       <c r="M17" s="40">
         <f ca="1"/>
-        <v>4.1086520947176686E-2</v>
+        <v>4.1084854014598507E-2</v>
       </c>
       <c r="N17" s="23">
         <f ca="1">_xll.qlYieldTSForwardRate(D$5,$D17,$D17,$D$1,"continuous","annual")</f>
-        <v>4.6999999997830312E-2</v>
+        <v>4.7000000000050744E-2</v>
       </c>
       <c r="P17" s="3">
         <f t="shared" ca="1" si="0"/>
@@ -1561,41 +1563,41 @@
       </c>
       <c r="R17" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>3.0768109536095656E-3</v>
+        <v>3.1064784794612166E-3</v>
       </c>
       <c r="S17" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>-1.1593806921675748E-3</v>
+        <v>-1.1724452554744899E-3</v>
       </c>
       <c r="T17" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>-1.0000000021696889E-3</v>
+        <v>-9.9999999994925676E-4</v>
       </c>
       <c r="U17" s="5"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="18">
         <f ca="1">_xll.qlDayCounterYearFraction($D$1,$D$8,D18)</f>
-        <v>4.0054794520547947</v>
+        <v>4.0082191780821921</v>
       </c>
       <c r="B18" s="19">
         <f t="shared" ca="1" si="6"/>
-        <v>0.99726027397260308</v>
+        <v>1.0054794520547947</v>
       </c>
       <c r="C18" s="43" t="s">
         <v>27</v>
       </c>
       <c r="D18" s="20">
         <f ca="1">_xll.qlCalendarAdvance($D$2,$D$8,C18)</f>
-        <v>43234</v>
+        <v>44536</v>
       </c>
       <c r="E18" s="21">
         <f t="shared" ca="1" si="5"/>
-        <v>0.83865934086012806</v>
+        <v>0.83848703130195046</v>
       </c>
       <c r="F18" s="22">
         <f ca="1">SUMPRODUCT($B$9:B18,$G$9:G18)/A18</f>
-        <v>4.3927496580027356E-2</v>
+        <v>4.3948735475051265E-2</v>
       </c>
       <c r="G18" s="23">
         <v>4.9000000000000002E-2</v>
@@ -1606,19 +1608,19 @@
       </c>
       <c r="J18" s="19">
         <f ca="1"/>
-        <v>4.0054794520547947</v>
+        <v>4.0082191780821921</v>
       </c>
       <c r="K18" s="20">
         <f ca="1"/>
-        <v>43234</v>
+        <v>44536</v>
       </c>
       <c r="L18" s="21">
         <f ca="1"/>
-        <v>0.84242911783827246</v>
+        <v>0.84229064772086704</v>
       </c>
       <c r="M18" s="40">
         <f ca="1"/>
-        <v>4.2807797537619686E-2</v>
+        <v>4.2819548872180459E-2</v>
       </c>
       <c r="N18" s="23">
         <f ca="1">_xll.qlYieldTSForwardRate(D$5,$D18,$D18,$D$1,"continuous","annual")</f>
@@ -1634,11 +1636,11 @@
       </c>
       <c r="R18" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>3.7697769781444013E-3</v>
+        <v>3.8036164189165778E-3</v>
       </c>
       <c r="S18" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>-1.1196990424076694E-3</v>
+        <v>-1.1291866028708061E-3</v>
       </c>
       <c r="T18" s="5">
         <f t="shared" ca="1" si="4"/>
@@ -1646,10 +1648,10 @@
       </c>
       <c r="U18" s="5"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="18">
         <f ca="1">_xll.qlDayCounterYearFraction($D$1,$D$8,D19)</f>
-        <v>5.0027397260273974</v>
+        <v>5.0054794520547947</v>
       </c>
       <c r="B19" s="19">
         <f t="shared" ca="1" si="6"/>
@@ -1660,15 +1662,15 @@
       </c>
       <c r="D19" s="20">
         <f ca="1">_xll.qlCalendarAdvance($D$2,$D$8,C19)</f>
-        <v>43598</v>
+        <v>44900</v>
       </c>
       <c r="E19" s="21">
         <f t="shared" ca="1" si="5"/>
-        <v>0.79826467108703014</v>
+        <v>0.79810066095075394</v>
       </c>
       <c r="F19" s="22">
         <f ca="1">SUMPRODUCT($B$9:B19,$G$9:G19)/A19</f>
-        <v>4.5038335158817083E-2</v>
+        <v>4.505473453749316E-2</v>
       </c>
       <c r="G19" s="23">
         <v>4.9500000000000002E-2</v>
@@ -1679,19 +1681,19 @@
       </c>
       <c r="J19" s="19">
         <f ca="1"/>
-        <v>5.0027397260273974</v>
+        <v>5.0054794520547947</v>
       </c>
       <c r="K19" s="20">
         <f ca="1"/>
-        <v>43598</v>
+        <v>44900</v>
       </c>
       <c r="L19" s="21">
         <f ca="1"/>
-        <v>0.80225280157649781</v>
+        <v>0.80212093524226169</v>
       </c>
       <c r="M19" s="40">
         <f ca="1"/>
-        <v>4.4042168674698776E-2</v>
+        <v>4.4050903119868638E-2</v>
       </c>
       <c r="N19" s="23">
         <f ca="1">_xll.qlYieldTSForwardRate(D$5,$D19,$D19,$D$1,"continuous","annual")</f>
@@ -1707,11 +1709,11 @@
       </c>
       <c r="R19" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>3.9881304894676672E-3</v>
+        <v>4.0202742915077527E-3</v>
       </c>
       <c r="S19" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>-9.9616648411830766E-4</v>
+        <v>-1.0038314176245219E-3</v>
       </c>
       <c r="T19" s="5">
         <f t="shared" ca="1" si="4"/>
@@ -1719,29 +1721,29 @@
       </c>
       <c r="U19" s="5"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="18">
         <f ca="1">_xll.qlDayCounterYearFraction($D$1,$D$8,D20)</f>
-        <v>6.0054794520547947</v>
+        <v>6.0027397260273974</v>
       </c>
       <c r="B20" s="19">
         <f t="shared" ca="1" si="6"/>
-        <v>1.0027397260273974</v>
+        <v>0.99726027397260264</v>
       </c>
       <c r="C20" s="43" t="s">
         <v>29</v>
       </c>
       <c r="D20" s="20">
         <f ca="1">_xll.qlCalendarAdvance($D$2,$D$8,C20)</f>
-        <v>43964</v>
+        <v>45264</v>
       </c>
       <c r="E20" s="21">
         <f t="shared" ca="1" si="5"/>
-        <v>0.75938110965504613</v>
+        <v>0.75943229158608216</v>
       </c>
       <c r="F20" s="22">
         <f ca="1">SUMPRODUCT($B$9:B20,$G$9:G20)/A20</f>
-        <v>4.5833394160583935E-2</v>
+        <v>4.5843085349155641E-2</v>
       </c>
       <c r="G20" s="23">
         <v>4.9799999999999997E-2</v>
@@ -1752,19 +1754,19 @@
       </c>
       <c r="J20" s="19">
         <f ca="1"/>
-        <v>6.0054794520547947</v>
+        <v>6.0027397260273974</v>
       </c>
       <c r="K20" s="20">
         <f ca="1"/>
-        <v>43964</v>
+        <v>45264</v>
       </c>
       <c r="L20" s="21">
         <f ca="1"/>
-        <v>0.76340459215745082</v>
+        <v>0.76348616577320783</v>
       </c>
       <c r="M20" s="40">
         <f ca="1"/>
-        <v>4.4953467153284681E-2</v>
+        <v>4.4956184390689186E-2</v>
       </c>
       <c r="N20" s="23">
         <f ca="1">_xll.qlYieldTSForwardRate(D$5,$D20,$D20,$D$1,"continuous","annual")</f>
@@ -1780,11 +1782,11 @@
       </c>
       <c r="R20" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>4.0234825024046961E-3</v>
+        <v>4.0538741871256612E-3</v>
       </c>
       <c r="S20" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>-8.7992700729925405E-4</v>
+        <v>-8.86900958466455E-4</v>
       </c>
       <c r="T20" s="5">
         <f t="shared" ca="1" si="4"/>
@@ -1792,29 +1794,29 @@
       </c>
       <c r="U20" s="5"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="18">
         <f ca="1">_xll.qlDayCounterYearFraction($D$1,$D$8,D21)</f>
         <v>7.0054794520547947</v>
       </c>
       <c r="B21" s="19">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>1.0027397260273974</v>
       </c>
       <c r="C21" s="43" t="s">
         <v>30</v>
       </c>
       <c r="D21" s="20">
         <f ca="1">_xll.qlCalendarAdvance($D$2,$D$8,C21)</f>
-        <v>44329</v>
+        <v>45630</v>
       </c>
       <c r="E21" s="21">
         <f t="shared" ca="1" si="5"/>
-        <v>0.72241789409132318</v>
+        <v>0.72236782138093025</v>
       </c>
       <c r="F21" s="22">
         <f ca="1">SUMPRODUCT($B$9:B21,$G$9:G21)/A21</f>
-        <v>4.6413883457176376E-2</v>
+        <v>4.6423777864685177E-2</v>
       </c>
       <c r="G21" s="23">
         <v>4.99E-2</v>
@@ -1829,15 +1831,15 @@
       </c>
       <c r="K21" s="20">
         <f ca="1"/>
-        <v>44329</v>
+        <v>45630</v>
       </c>
       <c r="L21" s="21">
         <f ca="1"/>
-        <v>0.72631815996573257</v>
+        <v>0.72629666922579539</v>
       </c>
       <c r="M21" s="40">
         <f ca="1"/>
-        <v>4.5645287446226049E-2</v>
+        <v>4.5649511145874067E-2</v>
       </c>
       <c r="N21" s="23">
         <f ca="1">_xll.qlYieldTSForwardRate(D$5,$D21,$D21,$D$1,"continuous","annual")</f>
@@ -1853,11 +1855,11 @@
       </c>
       <c r="R21" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>3.9002658744093921E-3</v>
+        <v>3.9288478448651354E-3</v>
       </c>
       <c r="S21" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>-7.6859601095032731E-4</v>
+        <v>-7.7426671881111048E-4</v>
       </c>
       <c r="T21" s="5">
         <f t="shared" ca="1" si="4"/>
@@ -1865,7 +1867,7 @@
       </c>
       <c r="U21" s="5"/>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="18">
         <f ca="1">_xll.qlDayCounterYearFraction($D$1,$D$8,D22)</f>
         <v>8.0054794520547947</v>
@@ -1879,15 +1881,15 @@
       </c>
       <c r="D22" s="20">
         <f ca="1">_xll.qlCalendarAdvance($D$2,$D$8,C22)</f>
-        <v>44694</v>
+        <v>45995</v>
       </c>
       <c r="E22" s="21">
         <f t="shared" ca="1" si="5"/>
-        <v>0.68718515764550714</v>
+        <v>0.68713752701001685</v>
       </c>
       <c r="F22" s="22">
         <f ca="1">SUMPRODUCT($B$9:B22,$G$9:G22)/A22</f>
-        <v>4.6861841204654343E-2</v>
+        <v>4.6870499657768648E-2</v>
       </c>
       <c r="G22" s="23">
         <v>0.05</v>
@@ -1902,19 +1904,19 @@
       </c>
       <c r="K22" s="20">
         <f ca="1"/>
-        <v>44694</v>
+        <v>45995</v>
       </c>
       <c r="L22" s="21">
         <f ca="1"/>
-        <v>0.69096429828374339</v>
+        <v>0.69094385361519617</v>
       </c>
       <c r="M22" s="40">
         <f ca="1"/>
-        <v>4.6176762491444215E-2</v>
+        <v>4.6180458590006843E-2</v>
       </c>
       <c r="N22" s="23">
         <f ca="1">_xll.qlYieldTSForwardRate(D$5,$D22,$D22,$D$1,"continuous","annual")</f>
-        <v>4.9950000001619095E-2</v>
+        <v>4.994999999939867E-2</v>
       </c>
       <c r="P22" s="3">
         <f t="shared" ca="1" si="0"/>
@@ -1926,41 +1928,41 @@
       </c>
       <c r="R22" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>3.7791406382362558E-3</v>
+        <v>3.8063266051793221E-3</v>
       </c>
       <c r="S22" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>-6.8507871321012853E-4</v>
+        <v>-6.9004106776180546E-4</v>
       </c>
       <c r="T22" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>-4.9999998380907684E-5</v>
+        <v>-5.0000000601332917E-5</v>
       </c>
       <c r="U22" s="5"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="18">
         <f ca="1">_xll.qlDayCounterYearFraction($D$1,$D$8,D23)</f>
-        <v>9.0109589041095894</v>
+        <v>9.0054794520547947</v>
       </c>
       <c r="B23" s="19">
         <f t="shared" ca="1" si="6"/>
-        <v>1.0054794520547947</v>
+        <v>1</v>
       </c>
       <c r="C23" s="43" t="s">
         <v>32</v>
       </c>
       <c r="D23" s="20">
         <f ca="1">_xll.qlCalendarAdvance($D$2,$D$8,C23)</f>
-        <v>45061</v>
+        <v>46360</v>
       </c>
       <c r="E23" s="21">
         <f t="shared" ca="1" si="5"/>
-        <v>0.65349167868838398</v>
+        <v>0.65362543437058218</v>
       </c>
       <c r="F23" s="22">
         <f ca="1">SUMPRODUCT($B$9:B23,$G$9:G23)/A23</f>
-        <v>4.7212009729401032E-2</v>
+        <v>4.7218010343778517E-2</v>
       </c>
       <c r="G23" s="23">
         <v>0.05</v>
@@ -1971,23 +1973,23 @@
       </c>
       <c r="J23" s="19">
         <f ca="1"/>
-        <v>9.0109589041095894</v>
+        <v>9.0054794520547947</v>
       </c>
       <c r="K23" s="20">
         <f ca="1"/>
-        <v>45061</v>
+        <v>46360</v>
       </c>
       <c r="L23" s="21">
         <f ca="1"/>
-        <v>0.65708552371283435</v>
+        <v>0.65724612423668871</v>
       </c>
       <c r="M23" s="40">
         <f ca="1"/>
-        <v>4.6603374885983595E-2</v>
+        <v>4.660459385457863E-2</v>
       </c>
       <c r="N23" s="23">
         <f ca="1">_xll.qlYieldTSForwardRate(D$5,$D23,$D23,$D$1,"continuous","annual")</f>
-        <v>5.0000000000129566E-2</v>
+        <v>5.0000000002349998E-2</v>
       </c>
       <c r="P23" s="3">
         <f t="shared" ca="1" si="0"/>
@@ -1999,41 +2001,41 @@
       </c>
       <c r="R23" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>3.5938450244503706E-3</v>
+        <v>3.6206898661065301E-3</v>
       </c>
       <c r="S23" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>-6.0863484341743684E-4</v>
+        <v>-6.134164891998875E-4</v>
       </c>
       <c r="T23" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>1.2956302697375577E-13</v>
+        <v>2.349995198436261E-12</v>
       </c>
       <c r="U23" s="5"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="18">
         <f ca="1">_xll.qlDayCounterYearFraction($D$1,$D$8,D24)</f>
-        <v>10.008219178082191</v>
+        <v>10.010958904109589</v>
       </c>
       <c r="B24" s="19">
         <f t="shared" ca="1" si="6"/>
-        <v>0.99726027397260175</v>
+        <v>1.0054794520547947</v>
       </c>
       <c r="C24" s="43" t="s">
         <v>33</v>
       </c>
       <c r="D24" s="20">
         <f ca="1">_xll.qlCalendarAdvance($D$2,$D$8,C24)</f>
-        <v>45425</v>
+        <v>46727</v>
       </c>
       <c r="E24" s="21">
         <f t="shared" ca="1" si="5"/>
-        <v>0.62170567276244559</v>
+        <v>0.62157742725956933</v>
       </c>
       <c r="F24" s="22">
         <f ca="1">SUMPRODUCT($B$9:B24,$G$9:G24)/A24</f>
-        <v>4.7489816589104845E-2</v>
+        <v>4.7497427476737818E-2</v>
       </c>
       <c r="G24" s="23">
         <v>0.05</v>
@@ -2044,19 +2046,19 @@
       </c>
       <c r="J24" s="19">
         <f ca="1"/>
-        <v>10.008219178082191</v>
+        <v>10.010958904109589</v>
       </c>
       <c r="K24" s="20">
         <f ca="1"/>
-        <v>45425</v>
+        <v>46727</v>
       </c>
       <c r="L24" s="21">
         <f ca="1"/>
-        <v>0.62512471222629062</v>
+        <v>0.62502059053556158</v>
       </c>
       <c r="M24" s="40">
         <f ca="1"/>
-        <v>4.6941828633999448E-2</v>
+        <v>4.6945621237000558E-2</v>
       </c>
       <c r="N24" s="23">
         <f ca="1">_xll.qlYieldTSForwardRate(D$5,$D24,$D24,$D$1,"continuous","annual")</f>
@@ -2072,11 +2074,11 @@
       </c>
       <c r="R24" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>3.4190394638450305E-3</v>
+        <v>3.4431632759922559E-3</v>
       </c>
       <c r="S24" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>-5.4798795510539733E-4</v>
+        <v>-5.5180623973725973E-4</v>
       </c>
       <c r="T24" s="5">
         <f t="shared" ca="1" si="4"/>
@@ -2084,10 +2086,10 @@
       </c>
       <c r="U24" s="5"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="18">
         <f ca="1">_xll.qlDayCounterYearFraction($D$1,$D$8,D25)</f>
-        <v>15.013698630136986</v>
+        <v>15.016438356164384</v>
       </c>
       <c r="B25" s="19">
         <f t="shared" ca="1" si="6"/>
@@ -2098,15 +2100,15 @@
       </c>
       <c r="D25" s="20">
         <f ca="1">_xll.qlCalendarAdvance($D$2,$D$8,C25)</f>
-        <v>47252</v>
+        <v>48554</v>
       </c>
       <c r="E25" s="21">
         <f t="shared" ca="1" si="5"/>
-        <v>0.48405222956975175</v>
+        <v>0.4839523792316911</v>
       </c>
       <c r="F25" s="22">
         <f ca="1">SUMPRODUCT($B$9:B25,$G$9:G25)/A25</f>
-        <v>4.8326697080291969E-2</v>
+        <v>4.8331618317825217E-2</v>
       </c>
       <c r="G25" s="23">
         <v>0.05</v>
@@ -2117,23 +2119,23 @@
       </c>
       <c r="J25" s="19">
         <f ca="1"/>
-        <v>15.013698630136986</v>
+        <v>15.016438356164384</v>
       </c>
       <c r="K25" s="20">
         <f ca="1"/>
-        <v>47252</v>
+        <v>48554</v>
       </c>
       <c r="L25" s="21">
         <f ca="1"/>
-        <v>0.48671425076075592</v>
+        <v>0.4866331829198916</v>
       </c>
       <c r="M25" s="40">
         <f ca="1"/>
-        <v>4.7961405109489062E-2</v>
+        <v>4.7963747491333704E-2</v>
       </c>
       <c r="N25" s="23">
         <f ca="1">_xll.qlYieldTSForwardRate(D$5,$D25,$D25,$D$1,"continuous","annual")</f>
-        <v>5.0000000000129566E-2</v>
+        <v>5.0000000002349998E-2</v>
       </c>
       <c r="P25" s="3">
         <f t="shared" ca="1" si="0"/>
@@ -2145,41 +2147,41 @@
       </c>
       <c r="R25" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>2.6620211910041713E-3</v>
+        <v>2.680803688200506E-3</v>
       </c>
       <c r="S25" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>-3.6529197080290704E-4</v>
+        <v>-3.6787082649151343E-4</v>
       </c>
       <c r="T25" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>1.2956302697375577E-13</v>
+        <v>2.349995198436261E-12</v>
       </c>
       <c r="U25" s="5"/>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="18">
         <f ca="1">_xll.qlDayCounterYearFraction($D$1,$D$8,D26)</f>
-        <v>20.019178082191782</v>
+        <v>20.013698630136986</v>
       </c>
       <c r="B26" s="19">
         <f t="shared" ca="1" si="6"/>
-        <v>5.0054794520547965</v>
+        <v>4.9972602739726018</v>
       </c>
       <c r="C26" s="43" t="s">
         <v>35</v>
       </c>
       <c r="D26" s="20">
         <f ca="1">_xll.qlCalendarAdvance($D$2,$D$8,C26)</f>
-        <v>49079</v>
+        <v>50378</v>
       </c>
       <c r="E26" s="21">
         <f t="shared" ca="1" si="5"/>
-        <v>0.39622159383791239</v>
+        <v>0.39627012038528436</v>
       </c>
       <c r="F26" s="22">
         <f ca="1">SUMPRODUCT($B$9:B26,$G$9:G26)/A26</f>
-        <v>4.6244737922540032E-2</v>
+        <v>4.6251279945242987E-2</v>
       </c>
       <c r="G26" s="23">
         <v>0.04</v>
@@ -2190,23 +2192,23 @@
       </c>
       <c r="J26" s="19">
         <f ca="1"/>
-        <v>20.019178082191782</v>
+        <v>20.013698630136986</v>
       </c>
       <c r="K26" s="20">
         <f ca="1"/>
-        <v>49079</v>
+        <v>50378</v>
       </c>
       <c r="L26" s="21">
         <f ca="1"/>
-        <v>0.37894960359182095</v>
+        <v>0.37904222396261739</v>
       </c>
       <c r="M26" s="40">
         <f ca="1"/>
-        <v>4.8471123580128651E-2</v>
+        <v>4.8472183436002743E-2</v>
       </c>
       <c r="N26" s="23">
         <f ca="1">_xll.qlYieldTSForwardRate(D$5,$D26,$D26,$D$1,"continuous","annual")</f>
-        <v>4.4999999999596196E-2</v>
+        <v>4.5000000001816629E-2</v>
       </c>
       <c r="P26" s="3">
         <f t="shared" ca="1" si="0"/>
@@ -2218,41 +2220,41 @@
       </c>
       <c r="R26" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>-1.727199024609144E-2</v>
+        <v>-1.7227896422666977E-2</v>
       </c>
       <c r="S26" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>2.2263856575886198E-3</v>
+        <v>2.2209034907597555E-3</v>
       </c>
       <c r="T26" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>4.9999999995961955E-3</v>
+        <v>5.0000000018166277E-3</v>
       </c>
       <c r="U26" s="5"/>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="18">
         <f ca="1">_xll.qlDayCounterYearFraction($D$1,$D$8,D27)</f>
         <v>25.016438356164382</v>
       </c>
       <c r="B27" s="19">
         <f t="shared" ca="1" si="6"/>
-        <v>4.9972602739726</v>
+        <v>5.0027397260273965</v>
       </c>
       <c r="C27" s="43" t="s">
         <v>36</v>
       </c>
       <c r="D27" s="20">
         <f ca="1">_xll.qlCalendarAdvance($D$2,$D$8,C27)</f>
-        <v>50903</v>
+        <v>52204</v>
       </c>
       <c r="E27" s="21">
         <f t="shared" ca="1" si="5"/>
-        <v>0.34105911735238248</v>
+        <v>0.34104482120134366</v>
       </c>
       <c r="F27" s="22">
         <f ca="1">SUMPRODUCT($B$9:B27,$G$9:G27)/A27</f>
-        <v>4.2999704304019282E-2</v>
+        <v>4.3001379914576726E-2</v>
       </c>
       <c r="G27" s="23">
         <v>0.03</v>
@@ -2267,19 +2269,19 @@
       </c>
       <c r="K27" s="20">
         <f ca="1"/>
-        <v>50903</v>
+        <v>52204</v>
       </c>
       <c r="L27" s="21">
         <f ca="1"/>
-        <v>0.31029169703367626</v>
+        <v>0.31029951818323748</v>
       </c>
       <c r="M27" s="40">
         <f ca="1"/>
-        <v>4.6778939875150589E-2</v>
+        <v>4.6777932318475525E-2</v>
       </c>
       <c r="N27" s="23">
         <f ca="1">_xll.qlYieldTSForwardRate(D$5,$D27,$D27,$D$1,"continuous","annual")</f>
-        <v>3.49999999991637E-2</v>
+        <v>3.5000000001384139E-2</v>
       </c>
       <c r="P27" s="3">
         <f t="shared" ca="1" si="0"/>
@@ -2291,41 +2293,41 @@
       </c>
       <c r="R27" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>-3.0767420318706218E-2</v>
+        <v>-3.0745303018106185E-2</v>
       </c>
       <c r="S27" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>3.7792355711313078E-3</v>
+        <v>3.7765524038987988E-3</v>
       </c>
       <c r="T27" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>4.9999999991637012E-3</v>
+        <v>5.0000000013841403E-3</v>
       </c>
       <c r="U27" s="5"/>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="24">
         <f ca="1">_xll.qlDayCounterYearFraction($D$1,$D$8,D28)</f>
-        <v>30.021917808219179</v>
+        <v>30.019178082191782</v>
       </c>
       <c r="B28" s="25">
         <f t="shared" ca="1" si="6"/>
-        <v>5.0054794520547965</v>
+        <v>5.0027397260274</v>
       </c>
       <c r="C28" s="43" t="s">
         <v>37</v>
       </c>
       <c r="D28" s="26">
         <f ca="1">_xll.qlCalendarAdvance($D$2,$D$8,C28)</f>
-        <v>52730</v>
+        <v>54030</v>
       </c>
       <c r="E28" s="27">
         <f t="shared" ca="1" si="5"/>
-        <v>0.30856923348335535</v>
+        <v>0.30857320686619039</v>
       </c>
       <c r="F28" s="28">
         <f ca="1">SUMPRODUCT($B$9:B28,$G$9:G28)/A28</f>
-        <v>3.9165020989231615E-2</v>
+        <v>3.916816646892398E-2</v>
       </c>
       <c r="G28" s="29">
         <v>0.02</v>
@@ -2336,23 +2338,23 @@
       </c>
       <c r="J28" s="25">
         <f ca="1"/>
-        <v>30.021917808219179</v>
+        <v>30.019178082191782</v>
       </c>
       <c r="K28" s="26">
         <f ca="1"/>
-        <v>52730</v>
+        <v>54030</v>
       </c>
       <c r="L28" s="27">
         <f ca="1"/>
-        <v>0.26702664025718464</v>
+        <v>0.26705531972678914</v>
       </c>
       <c r="M28" s="41">
         <f ca="1"/>
-        <v>4.3981429092900169E-2</v>
+        <v>4.3981865474126129E-2</v>
       </c>
       <c r="N28" s="29">
         <f ca="1">_xll.qlYieldTSForwardRate(D$5,$D28,$D28,$D$1,"continuous","annual")</f>
-        <v>2.5000000001805654E-2</v>
+        <v>2.4999999997364773E-2</v>
       </c>
       <c r="P28" s="3">
         <f t="shared" ca="1" si="0"/>
@@ -2364,19 +2366,19 @@
       </c>
       <c r="R28" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>-4.154259322617071E-2</v>
+        <v>-4.1517887139401244E-2</v>
       </c>
       <c r="S28" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>4.8164081036685541E-3</v>
+        <v>4.8136990052021489E-3</v>
       </c>
       <c r="T28" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>5.0000000018056538E-3</v>
+        <v>4.9999999973647721E-3</v>
       </c>
       <c r="U28" s="5"/>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="30"/>
       <c r="B29" s="31"/>
       <c r="C29" s="44" t="s">
@@ -2384,7 +2386,7 @@
       </c>
       <c r="D29" s="14">
         <f ca="1">_xll.qlCalendarAdvance($D$2,$D$8,C29)</f>
-        <v>53097</v>
+        <v>54396</v>
       </c>
       <c r="E29" s="31"/>
       <c r="F29" s="31"/>
@@ -2394,22 +2396,22 @@
       <c r="K29" s="31"/>
       <c r="L29" s="15">
         <f ca="1">_xll.qlYieldTSDiscount(D$5,$D29,TRUE)</f>
-        <v>0.26171047634590799</v>
+        <v>0.26175292707661302</v>
       </c>
       <c r="M29" s="39">
         <f ca="1">_xll.qlYieldTSZeroRate(D$5,$D29,$D$1,,,TRUE)</f>
-        <v>4.3204282560706408E-2</v>
+        <v>4.3206685507374373E-2</v>
       </c>
       <c r="N29" s="17">
         <f ca="1">_xll.qlYieldTSForwardRate(D$5,$D29,$D29,$D$1,"continuous","annual",TRUE)</f>
-        <v>1.9999999997898903E-2</v>
+        <v>2.0000000000119346E-2</v>
       </c>
       <c r="R29" s="4"/>
       <c r="S29" s="6"/>
       <c r="T29" s="5"/>
       <c r="U29" s="5"/>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="33"/>
       <c r="B30" s="34"/>
       <c r="C30" s="45" t="s">
@@ -2417,7 +2419,7 @@
       </c>
       <c r="D30" s="20">
         <f ca="1">_xll.qlCalendarAdvance($D$2,$D$8,C30)</f>
-        <v>54556</v>
+        <v>55857</v>
       </c>
       <c r="E30" s="34"/>
       <c r="F30" s="34"/>
@@ -2427,22 +2429,22 @@
       <c r="K30" s="34"/>
       <c r="L30" s="21">
         <f ca="1">_xll.qlYieldTSDiscount(D$5,$D30,TRUE)</f>
-        <v>0.24160245686363593</v>
+        <v>0.2416151661490602</v>
       </c>
       <c r="M30" s="40">
         <f ca="1">_xll.qlYieldTSZeroRate(D$5,$D30,$D$1,,,TRUE)</f>
-        <v>4.0556046620775978E-2</v>
+        <v>4.0554544743429295E-2</v>
       </c>
       <c r="N30" s="23">
         <f ca="1">_xll.qlYieldTSForwardRate(D$5,$D30,$D30,$D$1,"continuous","annual",TRUE)</f>
-        <v>2.0000000000119346E-2</v>
+        <v>1.9999999997898903E-2</v>
       </c>
       <c r="R30" s="4"/>
       <c r="S30" s="6"/>
       <c r="T30" s="5"/>
       <c r="U30" s="5"/>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="33"/>
       <c r="B31" s="34"/>
       <c r="C31" s="45" t="s">
@@ -2450,7 +2452,7 @@
       </c>
       <c r="D31" s="20">
         <f ca="1">_xll.qlCalendarAdvance($D$2,$D$8,C31)</f>
-        <v>56382</v>
+        <v>57683</v>
       </c>
       <c r="E31" s="34"/>
       <c r="F31" s="34"/>
@@ -2460,11 +2462,11 @@
       <c r="K31" s="34"/>
       <c r="L31" s="21">
         <f ca="1">_xll.qlYieldTSDiscount(D$5,$D31,TRUE)</f>
-        <v>0.21859896490599126</v>
+        <v>0.21861046411288884</v>
       </c>
       <c r="M31" s="40">
         <f ca="1">_xll.qlYieldTSZeroRate(D$5,$D31,$D$1,,,TRUE)</f>
-        <v>3.7986892539356609E-2</v>
+        <v>3.7985578370978781E-2</v>
       </c>
       <c r="N31" s="23">
         <f ca="1">_xll.qlYieldTSForwardRate(D$5,$D31,$D31,$D$1,"continuous","annual",TRUE)</f>
@@ -2475,7 +2477,7 @@
       <c r="T31" s="5"/>
       <c r="U31" s="5"/>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="33"/>
       <c r="B32" s="34"/>
       <c r="C32" s="45" t="s">
@@ -2483,7 +2485,7 @@
       </c>
       <c r="D32" s="20">
         <f ca="1">_xll.qlCalendarAdvance($D$2,$D$8,C32)</f>
-        <v>60035</v>
+        <v>61336</v>
       </c>
       <c r="E32" s="34"/>
       <c r="F32" s="34"/>
@@ -2493,22 +2495,22 @@
       <c r="K32" s="34"/>
       <c r="L32" s="21">
         <f ca="1">_xll.qlYieldTSDiscount(D$5,$D32,TRUE)</f>
-        <v>0.17894427724407572</v>
+        <v>0.17895369045089515</v>
       </c>
       <c r="M32" s="40">
         <f ca="1">_xll.qlYieldTSZeroRate(D$5,$D32,$D$1,,,TRUE)</f>
-        <v>3.4389120078847951E-2</v>
+        <v>3.4388068772928874E-2</v>
       </c>
       <c r="N32" s="23">
         <f ca="1">_xll.qlYieldTSForwardRate(D$5,$D32,$D32,$D$1,"continuous","annual",TRUE)</f>
-        <v>2.000000000678067E-2</v>
+        <v>1.9999999995678461E-2</v>
       </c>
       <c r="R32" s="4"/>
       <c r="S32" s="6"/>
       <c r="T32" s="5"/>
       <c r="U32" s="5"/>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="36"/>
       <c r="B33" s="37"/>
       <c r="C33" s="46" t="s">
@@ -2516,7 +2518,7 @@
       </c>
       <c r="D33" s="26">
         <f ca="1">_xll.qlCalendarAdvance($D$2,$D$8,C33)</f>
-        <v>63688</v>
+        <v>64990</v>
       </c>
       <c r="E33" s="37"/>
       <c r="F33" s="37"/>
@@ -2526,31 +2528,31 @@
       <c r="K33" s="37"/>
       <c r="L33" s="27">
         <f ca="1">_xll.qlYieldTSDiscount(D$5,$D33,TRUE)</f>
-        <v>0.14648310147385804</v>
+        <v>0.14648278041535739</v>
       </c>
       <c r="M33" s="41">
         <f ca="1">_xll.qlYieldTSZeroRate(D$5,$D33,$D$1,,,TRUE)</f>
-        <v>3.1990714546450083E-2</v>
+        <v>3.1989291417621024E-2</v>
       </c>
       <c r="N33" s="29">
         <f ca="1">_xll.qlYieldTSForwardRate(D$5,$D33,$D33,$D$1,"continuous","annual",TRUE)</f>
-        <v>2.0000000000119346E-2</v>
+        <v>1.9999999995678461E-2</v>
       </c>
       <c r="R33" s="4"/>
       <c r="S33" s="6"/>
       <c r="T33" s="5"/>
       <c r="U33" s="5"/>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D37" s="2"/>
     </row>
   </sheetData>

</xml_diff>